<commit_message>
updating lsoa lookup file
</commit_message>
<xml_diff>
--- a/6 neighbourhoods final option.xlsx
+++ b/6 neighbourhoods final option.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mapping Data\integrated health &amp; social care\neighbourhoods 9 to 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC89CF12-281B-40EE-97B1-418EE2CD991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDA93CF-4332-4E94-8551-BC84D955CEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsoa lookup" sheetId="1" r:id="rId1"/>
@@ -1441,24 +1441,6 @@
     <t>area name</t>
   </si>
   <si>
-    <t>1- Farnworth/ Kearsley</t>
-  </si>
-  <si>
-    <t>2 - Westhoughton/ Horwich</t>
-  </si>
-  <si>
-    <t>3 - Turton/ Belmont</t>
-  </si>
-  <si>
-    <t>4 - Breightmet/ Little Lever</t>
-  </si>
-  <si>
-    <t>5 - Town centre S</t>
-  </si>
-  <si>
-    <t>6 - Town centre N</t>
-  </si>
-  <si>
     <t>6 areas name</t>
   </si>
   <si>
@@ -1469,6 +1451,24 @@
   </si>
   <si>
     <t>Based on 2021/ 2011 LSOAs (no changes for Bolton)</t>
+  </si>
+  <si>
+    <t>2 - West</t>
+  </si>
+  <si>
+    <t>3 - North</t>
+  </si>
+  <si>
+    <t>4 - East</t>
+  </si>
+  <si>
+    <t>5 - Central S</t>
+  </si>
+  <si>
+    <t>6 - Central N</t>
+  </si>
+  <si>
+    <t>1 - South</t>
   </si>
 </sst>
 </file>
@@ -1795,11 +1795,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1830,10 +1830,10 @@
         <v>463</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="G2" t="str">
         <f>_xlfn.XLOOKUP(F2,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="G3" t="str">
         <f>_xlfn.XLOOKUP(F3,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="G4" t="str">
         <f>_xlfn.XLOOKUP(F4,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="G5" t="str">
         <f>_xlfn.XLOOKUP(F5,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="G6" t="str">
         <f>_xlfn.XLOOKUP(F6,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="G7" t="str">
         <f>_xlfn.XLOOKUP(F7,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="G8" t="str">
         <f>_xlfn.XLOOKUP(F8,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="G9" t="str">
         <f>_xlfn.XLOOKUP(F9,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="G10" t="str">
         <f>_xlfn.XLOOKUP(F10,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="G11" t="str">
         <f>_xlfn.XLOOKUP(F11,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="G12" t="str">
         <f>_xlfn.XLOOKUP(F12,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="G13" t="str">
         <f>_xlfn.XLOOKUP(F13,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="G14" t="str">
         <f>_xlfn.XLOOKUP(F14,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="G15" t="str">
         <f>_xlfn.XLOOKUP(F15,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="G16" t="str">
         <f>_xlfn.XLOOKUP(F16,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G17" t="str">
         <f>_xlfn.XLOOKUP(F17,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="G18" t="str">
         <f>_xlfn.XLOOKUP(F18,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="G19" t="str">
         <f>_xlfn.XLOOKUP(F19,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="G20" t="str">
         <f>_xlfn.XLOOKUP(F20,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="G21" t="str">
         <f>_xlfn.XLOOKUP(F21,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="G22" t="str">
         <f>_xlfn.XLOOKUP(F22,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G23" t="str">
         <f>_xlfn.XLOOKUP(F23,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="G24" t="str">
         <f>_xlfn.XLOOKUP(F24,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="G25" t="str">
         <f>_xlfn.XLOOKUP(F25,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="G26" t="str">
         <f>_xlfn.XLOOKUP(F26,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G27" t="str">
         <f>_xlfn.XLOOKUP(F27,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G28" t="str">
         <f>_xlfn.XLOOKUP(F28,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="G29" t="str">
         <f>_xlfn.XLOOKUP(F29,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="G30" t="str">
         <f>_xlfn.XLOOKUP(F30,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="G31" t="str">
         <f>_xlfn.XLOOKUP(F31,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="G32" t="str">
         <f>_xlfn.XLOOKUP(F32,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="G33" t="str">
         <f>_xlfn.XLOOKUP(F33,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="G34" t="str">
         <f>_xlfn.XLOOKUP(F34,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="G35" t="str">
         <f>_xlfn.XLOOKUP(F35,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="G36" t="str">
         <f>_xlfn.XLOOKUP(F36,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="G37" t="str">
         <f>_xlfn.XLOOKUP(F37,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="G38" t="str">
         <f>_xlfn.XLOOKUP(F38,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="G39" t="str">
         <f>_xlfn.XLOOKUP(F39,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="G40" t="str">
         <f>_xlfn.XLOOKUP(F40,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="G41" t="str">
         <f>_xlfn.XLOOKUP(F41,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="G42" t="str">
         <f>_xlfn.XLOOKUP(F42,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="G43" t="str">
         <f>_xlfn.XLOOKUP(F43,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="G44" t="str">
         <f>_xlfn.XLOOKUP(F44,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="G45" t="str">
         <f>_xlfn.XLOOKUP(F45,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="G46" t="str">
         <f>_xlfn.XLOOKUP(F46,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="G47" t="str">
         <f>_xlfn.XLOOKUP(F47,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="G48" t="str">
         <f>_xlfn.XLOOKUP(F48,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="G49" t="str">
         <f>_xlfn.XLOOKUP(F49,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="G50" t="str">
         <f>_xlfn.XLOOKUP(F50,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G51" t="str">
         <f>_xlfn.XLOOKUP(F51,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="G52" t="str">
         <f>_xlfn.XLOOKUP(F52,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="G53" t="str">
         <f>_xlfn.XLOOKUP(F53,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="G54" t="str">
         <f>_xlfn.XLOOKUP(F54,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="G55" t="str">
         <f>_xlfn.XLOOKUP(F55,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="G56" t="str">
         <f>_xlfn.XLOOKUP(F56,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="G57" t="str">
         <f>_xlfn.XLOOKUP(F57,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="G58" t="str">
         <f>_xlfn.XLOOKUP(F58,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G59" t="str">
         <f>_xlfn.XLOOKUP(F59,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="G60" t="str">
         <f>_xlfn.XLOOKUP(F60,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="G61" t="str">
         <f>_xlfn.XLOOKUP(F61,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="G62" t="str">
         <f>_xlfn.XLOOKUP(F62,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="G63" t="str">
         <f>_xlfn.XLOOKUP(F63,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="G64" t="str">
         <f>_xlfn.XLOOKUP(F64,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="G65" t="str">
         <f>_xlfn.XLOOKUP(F65,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="G66" t="str">
         <f>_xlfn.XLOOKUP(F66,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="G67" t="str">
         <f>_xlfn.XLOOKUP(F67,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="G68" t="str">
         <f>_xlfn.XLOOKUP(F68,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="G69" t="str">
         <f>_xlfn.XLOOKUP(F69,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="G70" t="str">
         <f>_xlfn.XLOOKUP(F70,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="G71" t="str">
         <f>_xlfn.XLOOKUP(F71,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="G72" t="str">
         <f>_xlfn.XLOOKUP(F72,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="G73" t="str">
         <f>_xlfn.XLOOKUP(F73,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="G74" t="str">
         <f>_xlfn.XLOOKUP(F74,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="G75" t="str">
         <f>_xlfn.XLOOKUP(F75,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="G76" t="str">
         <f>_xlfn.XLOOKUP(F76,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="G77" t="str">
         <f>_xlfn.XLOOKUP(F77,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="G78" t="str">
         <f>_xlfn.XLOOKUP(F78,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G79" t="str">
         <f>_xlfn.XLOOKUP(F79,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="G80" t="str">
         <f>_xlfn.XLOOKUP(F80,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="G81" t="str">
         <f>_xlfn.XLOOKUP(F81,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -3777,7 +3777,7 @@
       </c>
       <c r="G82" t="str">
         <f>_xlfn.XLOOKUP(F82,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="G83" t="str">
         <f>_xlfn.XLOOKUP(F83,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="G84" t="str">
         <f>_xlfn.XLOOKUP(F84,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="G85" t="str">
         <f>_xlfn.XLOOKUP(F85,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="G86" t="str">
         <f>_xlfn.XLOOKUP(F86,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="G87" t="str">
         <f>_xlfn.XLOOKUP(F87,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="G88" t="str">
         <f>_xlfn.XLOOKUP(F88,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="G89" t="str">
         <f>_xlfn.XLOOKUP(F89,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="G90" t="str">
         <f>_xlfn.XLOOKUP(F90,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="G91" t="str">
         <f>_xlfn.XLOOKUP(F91,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="G92" t="str">
         <f>_xlfn.XLOOKUP(F92,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="G93" t="str">
         <f>_xlfn.XLOOKUP(F93,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="G94" t="str">
         <f>_xlfn.XLOOKUP(F94,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="G95" t="str">
         <f>_xlfn.XLOOKUP(F95,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="G96" t="str">
         <f>_xlfn.XLOOKUP(F96,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="G97" t="str">
         <f>_xlfn.XLOOKUP(F97,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="G98" t="str">
         <f>_xlfn.XLOOKUP(F98,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="G99" t="str">
         <f>_xlfn.XLOOKUP(F99,names!A:A,names!B:B)</f>
-        <v>6 - Town centre N</v>
+        <v>6 - Central N</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="G100" t="str">
         <f>_xlfn.XLOOKUP(F100,names!A:A,names!B:B)</f>
-        <v>3 - Turton/ Belmont</v>
+        <v>3 - North</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="G101" t="str">
         <f>_xlfn.XLOOKUP(F101,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="G102" t="str">
         <f>_xlfn.XLOOKUP(F102,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
@@ -4281,7 +4281,7 @@
       </c>
       <c r="G103" t="str">
         <f>_xlfn.XLOOKUP(F103,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="G104" t="str">
         <f>_xlfn.XLOOKUP(F104,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="G105" t="str">
         <f>_xlfn.XLOOKUP(F105,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="G106" t="str">
         <f>_xlfn.XLOOKUP(F106,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="G107" t="str">
         <f>_xlfn.XLOOKUP(F107,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="G108" t="str">
         <f>_xlfn.XLOOKUP(F108,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="G109" t="str">
         <f>_xlfn.XLOOKUP(F109,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="G110" t="str">
         <f>_xlfn.XLOOKUP(F110,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="G111" t="str">
         <f>_xlfn.XLOOKUP(F111,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="G112" t="str">
         <f>_xlfn.XLOOKUP(F112,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="G113" t="str">
         <f>_xlfn.XLOOKUP(F113,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="G114" t="str">
         <f>_xlfn.XLOOKUP(F114,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="G115" t="str">
         <f>_xlfn.XLOOKUP(F115,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="G116" t="str">
         <f>_xlfn.XLOOKUP(F116,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="G117" t="str">
         <f>_xlfn.XLOOKUP(F117,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="G118" t="str">
         <f>_xlfn.XLOOKUP(F118,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -4665,7 +4665,7 @@
       </c>
       <c r="G119" t="str">
         <f>_xlfn.XLOOKUP(F119,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="G120" t="str">
         <f>_xlfn.XLOOKUP(F120,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="G121" t="str">
         <f>_xlfn.XLOOKUP(F121,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -4737,7 +4737,7 @@
       </c>
       <c r="G122" t="str">
         <f>_xlfn.XLOOKUP(F122,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="G123" t="str">
         <f>_xlfn.XLOOKUP(F123,names!A:A,names!B:B)</f>
-        <v>4 - Breightmet/ Little Lever</v>
+        <v>4 - East</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="G124" t="str">
         <f>_xlfn.XLOOKUP(F124,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="G125" t="str">
         <f>_xlfn.XLOOKUP(F125,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -4833,7 +4833,7 @@
       </c>
       <c r="G126" t="str">
         <f>_xlfn.XLOOKUP(F126,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="G127" t="str">
         <f>_xlfn.XLOOKUP(F127,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="G128" t="str">
         <f>_xlfn.XLOOKUP(F128,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
@@ -4905,7 +4905,7 @@
       </c>
       <c r="G129" t="str">
         <f>_xlfn.XLOOKUP(F129,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="G130" t="str">
         <f>_xlfn.XLOOKUP(F130,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="G131" t="str">
         <f>_xlfn.XLOOKUP(F131,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
@@ -4977,7 +4977,7 @@
       </c>
       <c r="G132" t="str">
         <f>_xlfn.XLOOKUP(F132,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -5001,7 +5001,7 @@
       </c>
       <c r="G133" t="str">
         <f>_xlfn.XLOOKUP(F133,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="G134" t="str">
         <f>_xlfn.XLOOKUP(F134,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="G135" t="str">
         <f>_xlfn.XLOOKUP(F135,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="G136" t="str">
         <f>_xlfn.XLOOKUP(F136,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="G137" t="str">
         <f>_xlfn.XLOOKUP(F137,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
@@ -5121,7 +5121,7 @@
       </c>
       <c r="G138" t="str">
         <f>_xlfn.XLOOKUP(F138,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
@@ -5145,7 +5145,7 @@
       </c>
       <c r="G139" t="str">
         <f>_xlfn.XLOOKUP(F139,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="G140" t="str">
         <f>_xlfn.XLOOKUP(F140,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
@@ -5193,7 +5193,7 @@
       </c>
       <c r="G141" t="str">
         <f>_xlfn.XLOOKUP(F141,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
@@ -5217,7 +5217,7 @@
       </c>
       <c r="G142" t="str">
         <f>_xlfn.XLOOKUP(F142,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="G143" t="str">
         <f>_xlfn.XLOOKUP(F143,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="G144" t="str">
         <f>_xlfn.XLOOKUP(F144,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="G145" t="str">
         <f>_xlfn.XLOOKUP(F145,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="G146" t="str">
         <f>_xlfn.XLOOKUP(F146,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -5337,7 +5337,7 @@
       </c>
       <c r="G147" t="str">
         <f>_xlfn.XLOOKUP(F147,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="G148" t="str">
         <f>_xlfn.XLOOKUP(F148,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="G149" t="str">
         <f>_xlfn.XLOOKUP(F149,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="G150" t="str">
         <f>_xlfn.XLOOKUP(F150,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
@@ -5433,7 +5433,7 @@
       </c>
       <c r="G151" t="str">
         <f>_xlfn.XLOOKUP(F151,names!A:A,names!B:B)</f>
-        <v>5 - Town centre S</v>
+        <v>5 - Central S</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="G152" t="str">
         <f>_xlfn.XLOOKUP(F152,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="G153" t="str">
         <f>_xlfn.XLOOKUP(F153,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
@@ -5505,7 +5505,7 @@
       </c>
       <c r="G154" t="str">
         <f>_xlfn.XLOOKUP(F154,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="G155" t="str">
         <f>_xlfn.XLOOKUP(F155,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
@@ -5553,7 +5553,7 @@
       </c>
       <c r="G156" t="str">
         <f>_xlfn.XLOOKUP(F156,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
@@ -5577,7 +5577,7 @@
       </c>
       <c r="G157" t="str">
         <f>_xlfn.XLOOKUP(F157,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
@@ -5601,7 +5601,7 @@
       </c>
       <c r="G158" t="str">
         <f>_xlfn.XLOOKUP(F158,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="G159" t="str">
         <f>_xlfn.XLOOKUP(F159,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
@@ -5649,7 +5649,7 @@
       </c>
       <c r="G160" t="str">
         <f>_xlfn.XLOOKUP(F160,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
@@ -5673,7 +5673,7 @@
       </c>
       <c r="G161" t="str">
         <f>_xlfn.XLOOKUP(F161,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="G162" t="str">
         <f>_xlfn.XLOOKUP(F162,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="G163" t="str">
         <f>_xlfn.XLOOKUP(F163,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
@@ -5745,7 +5745,7 @@
       </c>
       <c r="G164" t="str">
         <f>_xlfn.XLOOKUP(F164,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
@@ -5769,7 +5769,7 @@
       </c>
       <c r="G165" t="str">
         <f>_xlfn.XLOOKUP(F165,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
@@ -5793,7 +5793,7 @@
       </c>
       <c r="G166" t="str">
         <f>_xlfn.XLOOKUP(F166,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
@@ -5817,7 +5817,7 @@
       </c>
       <c r="G167" t="str">
         <f>_xlfn.XLOOKUP(F167,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="G168" t="str">
         <f>_xlfn.XLOOKUP(F168,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="G169" t="str">
         <f>_xlfn.XLOOKUP(F169,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
@@ -5889,7 +5889,7 @@
       </c>
       <c r="G170" t="str">
         <f>_xlfn.XLOOKUP(F170,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
@@ -5913,7 +5913,7 @@
       </c>
       <c r="G171" t="str">
         <f>_xlfn.XLOOKUP(F171,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="G172" t="str">
         <f>_xlfn.XLOOKUP(F172,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
@@ -5961,7 +5961,7 @@
       </c>
       <c r="G173" t="str">
         <f>_xlfn.XLOOKUP(F173,names!A:A,names!B:B)</f>
-        <v>1- Farnworth/ Kearsley</v>
+        <v>1 - South</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="G174" t="str">
         <f>_xlfn.XLOOKUP(F174,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="G175" t="str">
         <f>_xlfn.XLOOKUP(F175,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
@@ -6033,7 +6033,7 @@
       </c>
       <c r="G176" t="str">
         <f>_xlfn.XLOOKUP(F176,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
@@ -6057,7 +6057,7 @@
       </c>
       <c r="G177" t="str">
         <f>_xlfn.XLOOKUP(F177,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="G178" t="str">
         <f>_xlfn.XLOOKUP(F178,names!A:A,names!B:B)</f>
-        <v>2 - Westhoughton/ Horwich</v>
+        <v>2 - West</v>
       </c>
     </row>
   </sheetData>
@@ -6097,13 +6097,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -6119,7 +6119,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -6127,7 +6127,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -6135,7 +6135,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -6143,7 +6143,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -6151,7 +6151,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -6159,7 +6159,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -6171,7 +6171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4F8774-CF3E-40B2-B17B-86C0DBF64280}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -6179,12 +6179,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>